<commit_message>
Homework(Data Driven Framework for Registration)
</commit_message>
<xml_diff>
--- a/target/test-classes/LoginData.xlsx
+++ b/target/test-classes/LoginData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>Email</t>
   </si>
@@ -40,12 +40,16 @@
   </si>
   <si>
     <t>user101@gmail.com</t>
+  </si>
+  <si>
+    <t>Login(Login failed for invalid)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -392,8 +396,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="31.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="31.89453125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -446,6 +450,9 @@
       </c>
       <c r="B5">
         <v>123456</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>